<commit_message>
Recent re_pavane midi files.
</commit_message>
<xml_diff>
--- a/work/re_pavane.xlsx
+++ b/work/re_pavane.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="77">
   <si>
     <t>re_pavane_log_20151007</t>
     <phoneticPr fontId="1"/>
@@ -528,6 +528,132 @@
   </si>
   <si>
     <t>re_pavane_log_20151117b</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>re_pavane_log_20151119</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>★　　音数：低音少ない　わびさび　泣き　綺麗　やさしい</t>
+    <rPh sb="3" eb="4">
+      <t>オト</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>カズ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>テイオン</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>スク</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>キレイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>★〇　音数：少ない　わびさび　泣き　綺麗　やさしい　変奏感良</t>
+    <rPh sb="3" eb="4">
+      <t>オト</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>カズ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>スク</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>キレイ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ヘンソウ</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>カン</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>リョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>★〇　音数：低音少ない　わびさび　変わってる　変奏感　展開：面白い</t>
+    <rPh sb="3" eb="4">
+      <t>オト</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>カズ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>テイオン</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>スク</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ヘンソウ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>カン</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>テンカイ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>オモシロ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>★★　展開：巧み　かっこいい</t>
+    <rPh sb="3" eb="5">
+      <t>テンカイ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>タク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>★★　音数：少な目　展開：コンピュータらしい</t>
+    <rPh sb="3" eb="4">
+      <t>オト</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>カズ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>スク</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>メ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>テンカイ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -926,8 +1052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1426,7 +1552,9 @@
       <c r="J17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K17" s="1"/>
+      <c r="K17" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B18" s="1">
@@ -1456,7 +1584,9 @@
       <c r="J18" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K18" s="1"/>
+      <c r="K18" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B19" s="1">
@@ -1471,16 +1601,24 @@
       <c r="E19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="F19" s="1">
+        <v>0.34515732999999998</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0.3963888888888889</v>
+      </c>
       <c r="I19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K19" s="1"/>
+      <c r="K19" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B20" s="1">
@@ -1495,38 +1633,56 @@
       <c r="E20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="F20" s="1">
+        <v>0.30714032000000002</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" s="3">
+        <v>1.7415277777777778</v>
+      </c>
       <c r="I20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K20" s="1"/>
+      <c r="K20" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B21" s="1">
         <v>19</v>
       </c>
-      <c r="C21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="D21" s="1" t="s">
         <v>64</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="F21" s="1">
+        <v>0.24964330000000001</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0.39329861111111114</v>
+      </c>
       <c r="I21" s="1" t="s">
         <v>24</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K21" s="1"/>
+      <c r="K21" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B22" s="1">

</xml_diff>